<commit_message>
Updated spreadsheet writer library for original compatibility.
</commit_message>
<xml_diff>
--- a/RealmConverterTests/Assets/users.xlsx
+++ b/RealmConverterTests/Assets/users.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId4"/>
+    <sheet name="Dogs" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>idNumber</t>
   </si>
@@ -51,6 +52,33 @@
   </si>
   <si>
     <t>Lysander Down</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Fido</t>
+  </si>
+  <si>
+    <t>Rex</t>
+  </si>
+  <si>
+    <t>Scratchy</t>
+  </si>
+  <si>
+    <t>Itchy</t>
+  </si>
+  <si>
+    <t>Nikki</t>
+  </si>
+  <si>
+    <t>Scruffy</t>
+  </si>
+  <si>
+    <t>Floppy</t>
   </si>
 </sst>
 </file>
@@ -83,7 +111,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,8 +136,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -222,13 +262,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -256,6 +371,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +411,10 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1512,4 +1649,95 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="12" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.3828" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.3828" style="9" customWidth="1"/>
+    <col min="3" max="256" width="16.3516" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.75" customHeight="1">
+      <c r="A1" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="16.75" customHeight="1">
+      <c r="A2" t="s" s="11">
+        <v>15</v>
+      </c>
+      <c r="B2" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="16.55" customHeight="1">
+      <c r="A3" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="16.55" customHeight="1">
+      <c r="A4" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="B4" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" ht="16.55" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="16.55" customHeight="1">
+      <c r="A6" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" ht="16.55" customHeight="1">
+      <c r="A7" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="16.55" customHeight="1">
+      <c r="A8" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>